<commit_message>
Client registration almost done, to-do: transactions
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Numéro de carte</t>
   </si>
@@ -159,6 +159,45 @@
   </si>
   <si>
     <t>123123</t>
+  </si>
+  <si>
+    <t>953596</t>
+  </si>
+  <si>
+    <t>119511</t>
+  </si>
+  <si>
+    <t>Jihyeon Nam</t>
+  </si>
+  <si>
+    <t>658433</t>
+  </si>
+  <si>
+    <t>Kosuke Yokono</t>
+  </si>
+  <si>
+    <t>917859</t>
+  </si>
+  <si>
+    <t>Dahyeon Nam</t>
+  </si>
+  <si>
+    <t>153634</t>
+  </si>
+  <si>
+    <t>Celica Puth</t>
+  </si>
+  <si>
+    <t>598450</t>
+  </si>
+  <si>
+    <t>Vanita Puth</t>
+  </si>
+  <si>
+    <t>891090</t>
+  </si>
+  <si>
+    <t>Melissa Dupuch</t>
   </si>
 </sst>
 </file>
@@ -502,7 +541,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
@@ -820,6 +859,104 @@
         <v>0.0</v>
       </c>
       <c r="D22" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D29" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Partie bouton Achat et Terminer a continuer
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Numéro de carte</t>
   </si>
@@ -198,6 +198,15 @@
   </si>
   <si>
     <t>Melissa Dupuch</t>
+  </si>
+  <si>
+    <t>516122</t>
+  </si>
+  <si>
+    <t>683506</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -541,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
@@ -957,6 +966,34 @@
         <v>0.0</v>
       </c>
       <c r="D29" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D31" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A faire le sauvegarde dans fichier Excel
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Numéro de carte</t>
   </si>
@@ -152,61 +152,19 @@
     <t>252525</t>
   </si>
   <si>
-    <t>213415</t>
+    <t>364468</t>
+  </si>
+  <si>
+    <t>Kosuke Yokono</t>
+  </si>
+  <si>
+    <t>123123</t>
+  </si>
+  <si>
+    <t>584106</t>
   </si>
   <si>
     <t>Hana Murata</t>
-  </si>
-  <si>
-    <t>123123</t>
-  </si>
-  <si>
-    <t>953596</t>
-  </si>
-  <si>
-    <t>119511</t>
-  </si>
-  <si>
-    <t>Jihyeon Nam</t>
-  </si>
-  <si>
-    <t>658433</t>
-  </si>
-  <si>
-    <t>Kosuke Yokono</t>
-  </si>
-  <si>
-    <t>917859</t>
-  </si>
-  <si>
-    <t>Dahyeon Nam</t>
-  </si>
-  <si>
-    <t>153634</t>
-  </si>
-  <si>
-    <t>Celica Puth</t>
-  </si>
-  <si>
-    <t>598450</t>
-  </si>
-  <si>
-    <t>Vanita Puth</t>
-  </si>
-  <si>
-    <t>891090</t>
-  </si>
-  <si>
-    <t>Melissa Dupuch</t>
-  </si>
-  <si>
-    <t>516122</t>
-  </si>
-  <si>
-    <t>683506</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -550,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
@@ -876,124 +834,12 @@
         <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C23" t="n">
         <v>0.0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D31" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Manque juste les commentaires
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t>Numéro de carte</t>
   </si>
@@ -150,21 +150,6 @@
   </si>
   <si>
     <t>252525</t>
-  </si>
-  <si>
-    <t>364468</t>
-  </si>
-  <si>
-    <t>Kosuke Yokono</t>
-  </si>
-  <si>
-    <t>123123</t>
-  </si>
-  <si>
-    <t>584106</t>
-  </si>
-  <si>
-    <t>Hana Murata</t>
   </si>
 </sst>
 </file>
@@ -508,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
@@ -542,268 +527,268 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>40</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="C2" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>130</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C3" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>250</v>
-      </c>
-      <c r="D4">
-        <v>45.9</v>
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1234.9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1234.8900000000001</v>
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>458.99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>500</v>
-      </c>
-      <c r="D6">
-        <v>1234.9000000000001</v>
+        <v>6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>45.9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>710</v>
-      </c>
-      <c r="D7">
-        <v>34.369999999999997</v>
+        <v>13</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1890.34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>458.99</v>
+        <v>18</v>
+      </c>
+      <c r="C8" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>975</v>
-      </c>
-      <c r="D9">
-        <v>12.65</v>
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>130.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>260</v>
-      </c>
-      <c r="D10">
-        <v>400.09</v>
+        <v>21</v>
+      </c>
+      <c r="C10" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>120.0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1890.34</v>
+        <v>19</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>29</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="C12" t="n">
+        <v>710.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>34.37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>778</v>
-      </c>
-      <c r="D13">
-        <v>310.39999999999998</v>
+        <v>14</v>
+      </c>
+      <c r="C13" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14">
-        <v>140</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="C14" t="n">
+        <v>260.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>400.09</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>15</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="C15" t="n">
+        <v>975.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>12.65</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16">
-        <v>100</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="C17" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18">
-        <v>120</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="C18" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>250.0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19">
-        <v>200</v>
-      </c>
-      <c r="D19">
-        <v>120</v>
+        <v>7</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1234.89</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20">
-        <v>500</v>
-      </c>
-      <c r="D20">
-        <v>250</v>
+        <v>15</v>
+      </c>
+      <c r="C20" t="n">
+        <v>778.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>310.4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>45</v>
+      <c r="A21">
+        <v>123123</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
@@ -813,34 +798,6 @@
       </c>
       <c r="D21">
         <v>350</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>